<commit_message>
grid works; unaligned for different sheets
</commit_message>
<xml_diff>
--- a/Handwriting_Grid_Templates/handwriting_grid_template_dotted.xlsx
+++ b/Handwriting_Grid_Templates/handwriting_grid_template_dotted.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJ\Desktop\Computer_Vision_Finance_OCR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJ\Desktop\Computer_Vision_Finance_OCR\Handwriting_Grid_Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0457001A-97E0-4D2A-9C27-606713CFDD32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{030CA524-53FF-42DD-8BF9-6A9A4B482AD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="15375" windowHeight="8325" xr2:uid="{80B19C2B-4B9C-480C-B167-655CE597897C}"/>
+    <workbookView xWindow="2115" yWindow="10350" windowWidth="15375" windowHeight="8325" xr2:uid="{80B19C2B-4B9C-480C-B167-655CE597897C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -396,7 +396,7 @@
   <dimension ref="A1:AA36"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection sqref="A1:AA36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.42578125" defaultRowHeight="19.7" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>